<commit_message>
Ajuste data e hora
Ajuste data e hora
</commit_message>
<xml_diff>
--- a/ESP32.xlsx
+++ b/ESP32.xlsx
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>GND</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>RL5</t>
+  </si>
+  <si>
+    <t>RF</t>
   </si>
 </sst>
 </file>
@@ -255,7 +258,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,6 +313,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -390,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -426,6 +435,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -877,7 +889,7 @@
   <dimension ref="C3:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,6 +946,9 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="D8" s="2">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
troca do parametro porta RF
troca do parametro porta RF
</commit_message>
<xml_diff>
--- a/ESP32.xlsx
+++ b/ESP32.xlsx
@@ -399,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -438,6 +438,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -889,7 +892,7 @@
   <dimension ref="C3:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,7 +986,7 @@
       <c r="I10" s="2">
         <v>18</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="14" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>